<commit_message>
same name different content
</commit_message>
<xml_diff>
--- a/list-of-variables9.xlsx
+++ b/list-of-variables9.xlsx
@@ -67,219 +67,7 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"N° of Cases", "modifiers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:[{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">variable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Case Status", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Confirmed"}]}, {"alias":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Cases at onset of symptomps date", "variable":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N° of Cases", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">modifiers":[{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"variable":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"period type", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"value"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:"Onset of symptomps date"}]}]</t>
-    </r>
+    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"N° of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"N° of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -311,32 +99,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[{"15 days Incidence rate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
-    </r>
+    <t xml:space="preserve">[{"15 days Incidence rate":{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
   </si>
   <si>
     <t xml:space="preserve">Rt number</t>
@@ -754,7 +517,7 @@
     <t xml:space="preserve">Dashboard profile e.g. emergency</t>
   </si>
   <si>
-    <t xml:space="preserve">GDPR compliance</t>
+    <t xml:space="preserve">GDPR compliancess</t>
   </si>
 </sst>
 </file>
@@ -764,7 +527,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -785,11 +548,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -873,7 +631,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D101"/>
+      <selection pane="topLeft" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>